<commit_message>
ApachePOI Citizen functionality çözümü
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/Resource/ApacheExcel2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber7\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber8\src\test\java\ApachePOI\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="396" windowWidth="17280" windowHeight="8976" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,52 +63,52 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulais1145</t>
-  </si>
-  <si>
-    <t>ulais1146</t>
-  </si>
-  <si>
-    <t>ulais1147</t>
-  </si>
-  <si>
-    <t>ulais1148</t>
-  </si>
-  <si>
-    <t>ulais1149</t>
-  </si>
-  <si>
-    <t>ulais1150</t>
-  </si>
-  <si>
-    <t>ulais1151</t>
-  </si>
-  <si>
-    <t>ulais1152</t>
-  </si>
-  <si>
-    <t>urbs13</t>
-  </si>
-  <si>
-    <t>urbs14</t>
-  </si>
-  <si>
-    <t>urbs15</t>
-  </si>
-  <si>
-    <t>urbs16</t>
-  </si>
-  <si>
-    <t>urbs17</t>
-  </si>
-  <si>
-    <t>urbs18</t>
-  </si>
-  <si>
-    <t>urbs19</t>
-  </si>
-  <si>
-    <t>urbs20</t>
+    <t>ulais11451</t>
+  </si>
+  <si>
+    <t>ulais11462</t>
+  </si>
+  <si>
+    <t>ulais11473</t>
+  </si>
+  <si>
+    <t>ulais11483</t>
+  </si>
+  <si>
+    <t>ulais11494</t>
+  </si>
+  <si>
+    <t>ulais11505</t>
+  </si>
+  <si>
+    <t>ulais11516</t>
+  </si>
+  <si>
+    <t>ulais11527</t>
+  </si>
+  <si>
+    <t>urbs131</t>
+  </si>
+  <si>
+    <t>urbs141</t>
+  </si>
+  <si>
+    <t>urbs151</t>
+  </si>
+  <si>
+    <t>urbs161</t>
+  </si>
+  <si>
+    <t>urbs171</t>
+  </si>
+  <si>
+    <t>urbs181</t>
+  </si>
+  <si>
+    <t>urbs191</t>
+  </si>
+  <si>
+    <t>urbs201</t>
   </si>
 </sst>
 </file>
@@ -433,9 +433,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -481,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -512,16 +512,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -541,7 +541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -561,7 +561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -581,7 +581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -601,7 +601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -621,7 +621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -641,7 +641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -661,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>

</xml_diff>